<commit_message>
Window handle sample implementation
</commit_message>
<xml_diff>
--- a/target/classes/com/qa/practice/TestData/SeleniumPractice.xlsx
+++ b/target/classes/com/qa/practice/TestData/SeleniumPractice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antony/Desktop/Irin Study/Selenium/workspace/SeleniumPractice/src/main/java/com/qa/practice/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF77C28-4530-B84C-BD1C-D24132C137FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA4F6E8-3F48-AF4D-978E-5081CE9153BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15700" xr2:uid="{6CF24FF4-67AB-3045-B05D-F7A927551847}"/>
   </bookViews>
@@ -83,12 +83,6 @@
     <t>gfhfj</t>
   </si>
   <si>
-    <t>klln</t>
-  </si>
-  <si>
-    <t>ghjg</t>
-  </si>
-  <si>
     <t>jbblk</t>
   </si>
   <si>
@@ -99,6 +93,12 @@
   </si>
   <si>
     <t>Ruth</t>
+  </si>
+  <si>
+    <t>America</t>
+  </si>
+  <si>
+    <t>Srilanka</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -489,7 +489,7 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -506,10 +506,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -520,16 +520,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>

</xml_diff>